<commit_message>
Moved old draft to archive, and added current PsychoPy
</commit_message>
<xml_diff>
--- a/stim-faces.xlsx
+++ b/stim-faces.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,17 +448,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/2-Kasper-Surorg.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/24-Kobe-Bryant-(Lakers)-selected/$24-Kobe-Bryant.png</t>
         </is>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/33-Martin-Meiers.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/24-Kobe-Bryant-(Lakers)-selected/9-Matt-Barnes.png</t>
         </is>
       </c>
       <c r="B3" t="b">
@@ -468,7 +468,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/9-Severi-Kaukiainen.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/24-Kobe-Bryant-(Lakers)-selected/14-Troy-Murphy.png</t>
         </is>
       </c>
       <c r="B4" t="b">
@@ -478,17 +478,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/$11-Leemet-Bockler.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/24-Kobe-Bryant-(Lakers)-selected/15-Metta-World-Peace.png</t>
         </is>
       </c>
       <c r="B5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/15-Anrijs-Miska.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/24-Kobe-Bryant-(Lakers)-selected/16-Pau-Gasol.png</t>
         </is>
       </c>
       <c r="B6" t="b">
@@ -498,7 +498,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/$2-Cooper-Flagg.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/$11-Leemet-Bockler.png</t>
         </is>
       </c>
       <c r="B7" t="b">
@@ -508,7 +508,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/52-Stanley-Borden.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/2-Kasper-Surorg.png</t>
         </is>
       </c>
       <c r="B8" t="b">
@@ -518,7 +518,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/55-Spencer-Hubbard.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/33-Martin-Meiers.png</t>
         </is>
       </c>
       <c r="B9" t="b">
@@ -528,7 +528,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/7-Kon-Knueppel.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/9-Severi-Kaukiainen.png</t>
         </is>
       </c>
       <c r="B10" t="b">
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/8-Darren-Harris.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/11-Leemet-Bockler-(BC-Kalev)-selected/15-Anrijs-Miska.png</t>
         </is>
       </c>
       <c r="B11" t="b">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/$23-Stephanie-Mavunga.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/$2-Cooper-Flagg.png</t>
         </is>
       </c>
       <c r="B12" t="b">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/12-Liliana-Banaszak.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/52-Stanley-Borden.png</t>
         </is>
       </c>
       <c r="B13" t="b">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/13-Weronika-Gajda.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/55-Spencer-Hubbard.png</t>
         </is>
       </c>
       <c r="B14" t="b">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/15-Klaudia-Gertchen.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/7-Kon-Knueppel.png</t>
         </is>
       </c>
       <c r="B15" t="b">
@@ -588,7 +588,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/4-Julia-Niemojewska.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/2-Cooper-Flagg-(Duke-Blue-Devils)-selected/8-Darren-Harris.png</t>
         </is>
       </c>
       <c r="B16" t="b">
@@ -598,7 +598,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/$9-Marcelinho-Huertas.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/$23-Stephanie-Mavunga.png</t>
         </is>
       </c>
       <c r="B17" t="b">
@@ -608,7 +608,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/15-Joan-Sastre.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/12-Liliana-Banaszak.png</t>
         </is>
       </c>
       <c r="B18" t="b">
@@ -618,7 +618,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/3-Jaime-Fernandez.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/13-Weronika-Gajda.png</t>
         </is>
       </c>
       <c r="B19" t="b">
@@ -628,7 +628,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/35-Fran-Guerra.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/15-Klaudia-Gertchen.png</t>
         </is>
       </c>
       <c r="B20" t="b">
@@ -638,7 +638,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/42-Aaron-Doornekamp.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/23-Stephanie-Mavunga-(Poland)-selected/4-Julia-Niemojewska.png</t>
         </is>
       </c>
       <c r="B21" t="b">
@@ -648,7 +648,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/$9-Terezia-Palenikova.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/$9-Marcelinho-Huertas.png</t>
         </is>
       </c>
       <c r="B22" t="b">
@@ -658,7 +658,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/15-Nikola-Kovacikova.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/15-Joan-Sastre.png</t>
         </is>
       </c>
       <c r="B23" t="b">
@@ -668,7 +668,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/3-Ivana-Jakubcova.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/3-Jaime-Fernandez.png</t>
         </is>
       </c>
       <c r="B24" t="b">
@@ -678,7 +678,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/4-Veronika-Remenarova.png</t>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/35-Fran-Guerra.png</t>
         </is>
       </c>
       <c r="B25" t="b">
@@ -688,10 +688,60 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Marcelinho-Huertas-(La-Laguna-Tenerife)-selected/42-Aaron-Doornekamp.png</t>
+        </is>
+      </c>
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/$9-Terezia-Palenikova.png</t>
+        </is>
+      </c>
+      <c r="B27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/15-Nikola-Kovacikova.png</t>
+        </is>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/3-Ivana-Jakubcova.png</t>
+        </is>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/4-Veronika-Remenarova.png</t>
+        </is>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
           <t>C:\Users\diego\OneDrive\Documents\Coding\Neurotech\Neurocrime\Display/9-Terezia-Palenikova-(Slovakia)-selected/88-Natalia-Martiskova.png</t>
         </is>
       </c>
-      <c r="B26" t="b">
+      <c r="B31" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>